<commit_message>
added: 1. new training data set excel file. 2. refactored code into different files. 3. api integration.
</commit_message>
<xml_diff>
--- a/DecisionTree/wehealth.xlsx
+++ b/DecisionTree/wehealth.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naveens/Projects/datascience/DecisionTree/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sambasivap/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B4C21E-B132-7C47-9385-A66ED44503DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED7DB4B-638B-0F4E-B0EE-D900E290966E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{28E89936-AE41-5D45-9C74-D796D22053F0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16140" xr2:uid="{28E89936-AE41-5D45-9C74-D796D22053F0}"/>
   </bookViews>
   <sheets>
     <sheet name="wehealth" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="94">
   <si>
     <t>fever</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Skin rash</t>
   </si>
   <si>
-    <t>Dengu</t>
-  </si>
-  <si>
     <t>sore throat</t>
   </si>
   <si>
@@ -99,7 +96,223 @@
     <t>Disease</t>
   </si>
   <si>
-    <t>Loda</t>
+    <t>Dengue</t>
+  </si>
+  <si>
+    <t>Chickenpox</t>
+  </si>
+  <si>
+    <t>blisters</t>
+  </si>
+  <si>
+    <t>itching</t>
+  </si>
+  <si>
+    <t>Ringworm</t>
+  </si>
+  <si>
+    <t>problem with chewing</t>
+  </si>
+  <si>
+    <t>painful sores in mouth</t>
+  </si>
+  <si>
+    <t>skinredness</t>
+  </si>
+  <si>
+    <t>ringshaped-rash</t>
+  </si>
+  <si>
+    <t>Mouth ulcer</t>
+  </si>
+  <si>
+    <t>painful sores on tongue</t>
+  </si>
+  <si>
+    <t>irritation with spicy/sour foods</t>
+  </si>
+  <si>
+    <t>skin patches</t>
+  </si>
+  <si>
+    <t>indigestion</t>
+  </si>
+  <si>
+    <t>a feeling of fullness in your upper abdomen</t>
+  </si>
+  <si>
+    <t>gastritis</t>
+  </si>
+  <si>
+    <t>tarry stool</t>
+  </si>
+  <si>
+    <t>Burning eyes</t>
+  </si>
+  <si>
+    <t>Redness</t>
+  </si>
+  <si>
+    <t>discharge thick mucus from eye</t>
+  </si>
+  <si>
+    <t>Conjuctivities</t>
+  </si>
+  <si>
+    <t>Itchy eyes</t>
+  </si>
+  <si>
+    <t>More tears than usual</t>
+  </si>
+  <si>
+    <t>Cough</t>
+  </si>
+  <si>
+    <t>wheezing</t>
+  </si>
+  <si>
+    <t>chest tightness</t>
+  </si>
+  <si>
+    <t>breathlessness</t>
+  </si>
+  <si>
+    <t>phlegm</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
+    <t>nausea</t>
+  </si>
+  <si>
+    <t>sweating</t>
+  </si>
+  <si>
+    <t>chest pain</t>
+  </si>
+  <si>
+    <t>pain spreads to your arms, jaws etc</t>
+  </si>
+  <si>
+    <t>Coronary Heart Disease</t>
+  </si>
+  <si>
+    <t>high bp</t>
+  </si>
+  <si>
+    <t>pain in jaws that radiates to chest</t>
+  </si>
+  <si>
+    <t>increase in heart beat</t>
+  </si>
+  <si>
+    <t>more burping than usual</t>
+  </si>
+  <si>
+    <t>fainting spells</t>
+  </si>
+  <si>
+    <t>dehydration</t>
+  </si>
+  <si>
+    <t>weight gain</t>
+  </si>
+  <si>
+    <t>Fatigue</t>
+  </si>
+  <si>
+    <t>Weakness</t>
+  </si>
+  <si>
+    <t>Muscle aches and cramps</t>
+  </si>
+  <si>
+    <t>Eye and face swelling</t>
+  </si>
+  <si>
+    <t>Increased blood cholesterol levels</t>
+  </si>
+  <si>
+    <t>Constipation</t>
+  </si>
+  <si>
+    <t>Weight gain</t>
+  </si>
+  <si>
+    <t>Weight loss</t>
+  </si>
+  <si>
+    <t>HypoThyroidism</t>
+  </si>
+  <si>
+    <t>Skin thinning</t>
+  </si>
+  <si>
+    <t>Nervousness</t>
+  </si>
+  <si>
+    <t>Racing heartbeat or palpitations</t>
+  </si>
+  <si>
+    <t>HyperThyroidism</t>
+  </si>
+  <si>
+    <t>hair loss</t>
+  </si>
+  <si>
+    <t>poor appetite</t>
+  </si>
+  <si>
+    <t>more hunger than usual</t>
+  </si>
+  <si>
+    <t>Frequent Urination</t>
+  </si>
+  <si>
+    <t>Tingling, numbness, or pain in the hands or feet</t>
+  </si>
+  <si>
+    <t>Type 2 Diabetes</t>
+  </si>
+  <si>
+    <t>blurry vision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fatigue </t>
+  </si>
+  <si>
+    <t>Irregular heartbeat</t>
+  </si>
+  <si>
+    <t>Pounding in your chest, neck, or ears</t>
+  </si>
+  <si>
+    <t>Chest pain</t>
+  </si>
+  <si>
+    <t>Hyper Tension</t>
+  </si>
+  <si>
+    <t>Blood spots in the eyes</t>
+  </si>
+  <si>
+    <t>Dizziness</t>
+  </si>
+  <si>
+    <t>nosebleeds</t>
+  </si>
+  <si>
+    <t>cold skin</t>
+  </si>
+  <si>
+    <t>Low Blood Pressure</t>
+  </si>
+  <si>
+    <t>Lightheadedness</t>
+  </si>
+  <si>
+    <t>Nausea</t>
   </si>
 </sst>
 </file>
@@ -466,36 +679,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8CB8AE-61A1-2B4B-9E86-36D32B203EC0}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -535,7 +751,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -543,19 +759,19 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -563,19 +779,19 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -592,15 +808,15 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -609,13 +825,581 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" t="s">
+        <v>73</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" t="s">
+        <v>88</v>
+      </c>
+      <c r="F34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>